<commit_message>
Registration and Login without listener and assertion
</commit_message>
<xml_diff>
--- a/com.Demowebshop/src/test/resources/TestData/DemowebshopTestData.xlsx
+++ b/com.Demowebshop/src/test/resources/TestData/DemowebshopTestData.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\git\EcommerceProject\com.Demowebshop\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB78657-879C-4722-938A-E4864AE22A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D2E42B-2236-464C-90A2-E3B1DD4D1B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CA6FA5AE-493D-4403-85B4-72E077E9AFBD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CA6FA5AE-493D-4403-85B4-72E077E9AFBD}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterData" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginDataAfterReg" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>First Name</t>
   </si>
@@ -50,17 +51,87 @@
     <t>Deepak</t>
   </si>
   <si>
-    <t>Kalal</t>
-  </si>
-  <si>
     <t>Kalal@123</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>Preeti</t>
+  </si>
+  <si>
+    <t>Krishna</t>
+  </si>
+  <si>
+    <t>Pooja</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Naina</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Rajeev</t>
+  </si>
+  <si>
+    <t>Pranya</t>
+  </si>
+  <si>
+    <t>Verma</t>
+  </si>
+  <si>
+    <t>Arora</t>
+  </si>
+  <si>
+    <t>Bisht</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Bhardwaj</t>
+  </si>
+  <si>
+    <t>Nautiyal</t>
+  </si>
+  <si>
+    <t>Sandhu</t>
+  </si>
+  <si>
+    <t>Kriti</t>
+  </si>
+  <si>
+    <t>Goyal</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PriyaGoyal878@testxp.com</t>
+  </si>
+  <si>
+    <t>Goyal@123</t>
+  </si>
+  <si>
+    <t>KritiNautiyal5868@testxp.com</t>
+  </si>
+  <si>
+    <t>Nautiyal@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,12 +150,25 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,6 +178,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -122,22 +212,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{20B7860F-2368-4EAC-B047-685855B61C49}"/>
   </cellStyles>
@@ -471,15 +568,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA575E51-580D-480E-8910-878805A4405D}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.6640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="16.44140625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -498,10 +597,120 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{06962281-3C96-4DA0-879D-565A4B1648AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14162E26-2E2E-4241-9FFB-94C488696BA7}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="28.77734375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6th April final commit with extent Report
</commit_message>
<xml_diff>
--- a/com.Demowebshop/src/test/resources/TestData/DemowebshopTestData.xlsx
+++ b/com.Demowebshop/src/test/resources/TestData/DemowebshopTestData.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>First Name</t>
   </si>
@@ -167,6 +167,63 @@
   </si>
   <si>
     <t>Sharma@123</t>
+  </si>
+  <si>
+    <t>DeepakSharma8816@testxp.com</t>
+  </si>
+  <si>
+    <t>RahulGoyal5711@testxp.com</t>
+  </si>
+  <si>
+    <t>RahulGoyal943@testxp.com</t>
+  </si>
+  <si>
+    <t>RajeevSingh7882@testxp.com</t>
+  </si>
+  <si>
+    <t>Singh@123</t>
+  </si>
+  <si>
+    <t>PriyaSharma3289@testxp.com</t>
+  </si>
+  <si>
+    <t>KrishnaNautiyal5934@testxp.com</t>
+  </si>
+  <si>
+    <t>PoojaGoyal665@testxp.com</t>
+  </si>
+  <si>
+    <t>KritiSandhu5771@testxp.com</t>
+  </si>
+  <si>
+    <t>Sandhu@123</t>
+  </si>
+  <si>
+    <t>PriyaSharma8638@testxp.com</t>
+  </si>
+  <si>
+    <t>PriyaSharma1927@testxp.com</t>
+  </si>
+  <si>
+    <t>NainaBisht1323@testxp.com</t>
+  </si>
+  <si>
+    <t>Bisht@123</t>
+  </si>
+  <si>
+    <t>RahulSingh1336@testxp.com</t>
+  </si>
+  <si>
+    <t>DeepakBhardwaj1044@testxp.com</t>
+  </si>
+  <si>
+    <t>Bhardwaj@123</t>
+  </si>
+  <si>
+    <t>KritiSandhu3738@testxp.com</t>
+  </si>
+  <si>
+    <t>NainaArora6462@testxp.com</t>
   </si>
 </sst>
 </file>
@@ -750,10 +807,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>